<commit_message>
Update benchmarks in readme
</commit_message>
<xml_diff>
--- a/Docs/MeasurementsBenchmarks.xlsx
+++ b/Docs/MeasurementsBenchmarks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\prometheus-net\prometheus-net\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFFC146A-5B01-4734-BA23-6BC68334CB8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8263AE41-25B5-4686-A946-C0A01E1F93DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12690" yWindow="-16185" windowWidth="28770" windowHeight="15570" xr2:uid="{85E95B3F-98C7-440F-904A-790DCCCB2201}"/>
+    <workbookView xWindow="28695" yWindow="0" windowWidth="29010" windowHeight="23505" xr2:uid="{85E95B3F-98C7-440F-904A-790DCCCB2201}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -102,7 +102,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -122,9 +122,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -162,7 +162,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -268,7 +268,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -410,7 +410,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -421,7 +421,7 @@
   <dimension ref="B2:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,106 +454,106 @@
         <v>200000</v>
       </c>
       <c r="G3">
-        <v>2295</v>
+        <v>385</v>
       </c>
       <c r="H3">
         <f>G3/1000</f>
-        <v>2.2949999999999999</v>
+        <v>0.38500000000000001</v>
       </c>
       <c r="I3" s="1">
         <f>1000/H3*$C$3</f>
-        <v>87145969.49891068</v>
+        <v>519480519.48051941</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="G4">
-        <v>384</v>
+        <v>1497</v>
       </c>
       <c r="H4">
         <f t="shared" ref="H4:H10" si="0">G4/1000</f>
-        <v>0.38400000000000001</v>
+        <v>1.4970000000000001</v>
       </c>
       <c r="I4" s="1">
-        <f t="shared" ref="I4:I10" si="1">1000/H4*$C$3</f>
-        <v>520833333.33333331</v>
+        <f t="shared" ref="I4:I6" si="1">1000/H4*$C$3</f>
+        <v>133600534.40213761</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="G5">
-        <v>4331</v>
+        <v>2880</v>
       </c>
       <c r="H5">
         <f t="shared" si="0"/>
-        <v>4.3310000000000004</v>
+        <v>2.88</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" si="1"/>
-        <v>46178711.613945968</v>
+        <v>69444444.444444448</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="G6">
-        <v>82126</v>
+        <v>80006</v>
       </c>
       <c r="H6">
         <f t="shared" si="0"/>
-        <v>82.126000000000005</v>
+        <v>80.006</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="1"/>
-        <v>2435282.3709909162</v>
+        <v>2499812.5140614454</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="G7">
-        <v>325485</v>
+        <v>60615</v>
       </c>
       <c r="H7">
-        <f t="shared" si="0"/>
-        <v>325.48500000000001</v>
+        <f>G7/1000</f>
+        <v>60.615000000000002</v>
       </c>
       <c r="J7" s="1">
         <f>1000/H7*$C$3*16</f>
-        <v>9831482.2495660316</v>
+        <v>52792213.148560584</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="G8">
-        <v>58076</v>
+        <v>366126</v>
       </c>
       <c r="H8">
-        <f t="shared" si="0"/>
-        <v>58.076000000000001</v>
+        <f>G8/1000</f>
+        <v>366.12599999999998</v>
       </c>
       <c r="J8" s="1">
         <f t="shared" ref="J8:J10" si="2">1000/H8*$C$3*16</f>
-        <v>55100213.513327368</v>
+        <v>8740160.4911970198</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="G9">
-        <v>234004</v>
+        <v>579632</v>
       </c>
       <c r="H9">
         <f t="shared" si="0"/>
-        <v>234.00399999999999</v>
+        <v>579.63199999999995</v>
       </c>
       <c r="J9" s="1">
         <f t="shared" si="2"/>
-        <v>13674979.91487325</v>
+        <v>5520744.1963176643</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="G10">
-        <v>1751999</v>
+        <v>1749837</v>
       </c>
       <c r="H10">
         <f t="shared" si="0"/>
-        <v>1751.999</v>
+        <v>1749.837</v>
       </c>
       <c r="J10" s="1">
         <f t="shared" si="2"/>
-        <v>1826485.0607791441</v>
+        <v>1828741.7628041925</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update benchmark results in readme
</commit_message>
<xml_diff>
--- a/Docs/MeasurementsBenchmarks.xlsx
+++ b/Docs/MeasurementsBenchmarks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\prometheus-net\prometheus-net\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8263AE41-25B5-4686-A946-C0A01E1F93DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33EC4C82-158F-4F04-B1E1-8E994EADCDDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="0" windowWidth="29010" windowHeight="23505" xr2:uid="{85E95B3F-98C7-440F-904A-790DCCCB2201}"/>
+    <workbookView xWindow="26985" yWindow="-15525" windowWidth="28500" windowHeight="15435" xr2:uid="{85E95B3F-98C7-440F-904A-790DCCCB2201}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Measurements</t>
   </si>
@@ -47,10 +47,7 @@
     <t>ms</t>
   </si>
   <si>
-    <t>per sec total 1T</t>
-  </si>
-  <si>
-    <t>per sec total 16T</t>
+    <t>per sec</t>
   </si>
 </sst>
 </file>
@@ -418,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{175044FC-35C8-41C4-AA64-A6014973B48C}">
-  <dimension ref="B2:J10"/>
+  <dimension ref="B2:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -432,7 +429,7 @@
     <col min="10" max="10" width="16.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="G2" t="s">
         <v>1</v>
       </c>
@@ -442,118 +439,63 @@
       <c r="I2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>4</v>
-      </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
       <c r="C3">
-        <v>200000</v>
+        <v>100000</v>
       </c>
       <c r="G3">
-        <v>385</v>
+        <v>385.6</v>
       </c>
       <c r="H3">
         <f>G3/1000</f>
-        <v>0.38500000000000001</v>
+        <v>0.3856</v>
       </c>
       <c r="I3" s="1">
         <f>1000/H3*$C$3</f>
-        <v>519480519.48051941</v>
+        <v>259336099.58506221</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="G4">
-        <v>1497</v>
+        <v>168.7</v>
       </c>
       <c r="H4">
         <f t="shared" ref="H4:H10" si="0">G4/1000</f>
-        <v>1.4970000000000001</v>
+        <v>0.16869999999999999</v>
       </c>
       <c r="I4" s="1">
-        <f t="shared" ref="I4:I6" si="1">1000/H4*$C$3</f>
-        <v>133600534.40213761</v>
+        <f t="shared" ref="I4:I7" si="1">1000/H4*$C$3</f>
+        <v>592768227.62299943</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="G5">
-        <v>2880</v>
+        <v>940.9</v>
       </c>
       <c r="H5">
         <f t="shared" si="0"/>
-        <v>2.88</v>
+        <v>0.94089999999999996</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" si="1"/>
-        <v>69444444.444444448</v>
+        <v>106281220.10840684</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="G6">
-        <v>80006</v>
+        <v>1728</v>
       </c>
       <c r="H6">
         <f t="shared" si="0"/>
-        <v>80.006</v>
+        <v>1.728</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="1"/>
-        <v>2499812.5140614454</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="G7">
-        <v>60615</v>
-      </c>
-      <c r="H7">
-        <f>G7/1000</f>
-        <v>60.615000000000002</v>
-      </c>
-      <c r="J7" s="1">
-        <f>1000/H7*$C$3*16</f>
-        <v>52792213.148560584</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="G8">
-        <v>366126</v>
-      </c>
-      <c r="H8">
-        <f>G8/1000</f>
-        <v>366.12599999999998</v>
-      </c>
-      <c r="J8" s="1">
-        <f t="shared" ref="J8:J10" si="2">1000/H8*$C$3*16</f>
-        <v>8740160.4911970198</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="G9">
-        <v>579632</v>
-      </c>
-      <c r="H9">
-        <f t="shared" si="0"/>
-        <v>579.63199999999995</v>
-      </c>
-      <c r="J9" s="1">
-        <f t="shared" si="2"/>
-        <v>5520744.1963176643</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="G10">
-        <v>1749837</v>
-      </c>
-      <c r="H10">
-        <f t="shared" si="0"/>
-        <v>1749.837</v>
-      </c>
-      <c r="J10" s="1">
-        <f t="shared" si="2"/>
-        <v>1828741.7628041925</v>
+        <v>57870370.370370373</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Use slightly maybe sort of a bit faster atomic logic in random places
Seems to benefit exemplar case the most?
</commit_message>
<xml_diff>
--- a/Docs/MeasurementsBenchmarks.xlsx
+++ b/Docs/MeasurementsBenchmarks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\prometheus-net\prometheus-net\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33EC4C82-158F-4F04-B1E1-8E994EADCDDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DDE987E-C893-438B-8A66-3E67936B9100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26985" yWindow="-15525" windowWidth="28500" windowHeight="15435" xr2:uid="{85E95B3F-98C7-440F-904A-790DCCCB2201}"/>
+    <workbookView xWindow="22170" yWindow="4770" windowWidth="28500" windowHeight="15435" xr2:uid="{85E95B3F-98C7-440F-904A-790DCCCB2201}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -418,7 +418,7 @@
   <dimension ref="B2:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,54 +448,54 @@
         <v>100000</v>
       </c>
       <c r="G3">
-        <v>385.6</v>
+        <v>383.5</v>
       </c>
       <c r="H3">
         <f>G3/1000</f>
-        <v>0.3856</v>
+        <v>0.38350000000000001</v>
       </c>
       <c r="I3" s="1">
         <f>1000/H3*$C$3</f>
-        <v>259336099.58506221</v>
+        <v>260756192.95958278</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="G4">
-        <v>168.7</v>
+        <v>169.1</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:H10" si="0">G4/1000</f>
-        <v>0.16869999999999999</v>
+        <f t="shared" ref="H4:H6" si="0">G4/1000</f>
+        <v>0.1691</v>
       </c>
       <c r="I4" s="1">
-        <f t="shared" ref="I4:I7" si="1">1000/H4*$C$3</f>
-        <v>592768227.62299943</v>
+        <f t="shared" ref="I4:I6" si="1">1000/H4*$C$3</f>
+        <v>591366055.58840919</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="G5">
-        <v>940.9</v>
+        <v>953.5</v>
       </c>
       <c r="H5">
         <f t="shared" si="0"/>
-        <v>0.94089999999999996</v>
+        <v>0.95350000000000001</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" si="1"/>
-        <v>106281220.10840684</v>
+        <v>104876769.79549031</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="G6">
-        <v>1728</v>
+        <v>1531.1</v>
       </c>
       <c r="H6">
         <f t="shared" si="0"/>
-        <v>1.728</v>
+        <v>1.5310999999999999</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="1"/>
-        <v>57870370.370370373</v>
+        <v>65312520.410162628</v>
       </c>
     </row>
   </sheetData>

</xml_diff>